<commit_message>
Solicitudes Info NAMAs - Actualizado a Junio 2023
</commit_message>
<xml_diff>
--- a/Estadísticas Solicitudes Información NAMAs, CNCCDL, 2019.xlsx
+++ b/Estadísticas Solicitudes Información NAMAs, CNCCDL, 2019.xlsx
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="17">
   <si>
     <t xml:space="preserve">Mes</t>
   </si>
   <si>
-    <t xml:space="preserve">Solicitudes_Información_Recibidas</t>
+    <t xml:space="preserve">Solicitudes_Informaci�n_Recibidas</t>
   </si>
   <si>
     <t xml:space="preserve">Respondidas</t>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">En_Proceso</t>
   </si>
   <si>
-    <t xml:space="preserve">Año</t>
+    <t xml:space="preserve">A�o</t>
   </si>
   <si>
     <t xml:space="preserve">Enero</t>
@@ -166,16 +166,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G47" activeCellId="0" sqref="G47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H48" activeCellId="0" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.47"/>
@@ -1012,6 +1012,108 @@
       </c>
       <c r="E49" s="0" t="n">
         <v>2022</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <v>2023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>